<commit_message>
nev data - 23.01.2023 17:24:07,07
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -214,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,23 +287,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,7 +375,7 @@
   <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD42" activeCellId="0" sqref="AD42"/>
+      <selection pane="topLeft" activeCell="Y18" activeCellId="0" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -905,7 +893,7 @@
         <f aca="false">AH7*$AL4</f>
         <v>20160</v>
       </c>
-      <c r="AM7" s="18" t="n">
+      <c r="AM7" s="15" t="n">
         <f aca="false">AJ7+5000</f>
         <v>18116</v>
       </c>
@@ -1017,7 +1005,7 @@
       </c>
       <c r="AJ8" s="15"/>
       <c r="AK8" s="15"/>
-      <c r="AM8" s="18"/>
+      <c r="AM8" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
@@ -1035,7 +1023,7 @@
       <c r="E10" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="F10" s="19" t="n">
+      <c r="F10" s="18" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="5" t="n">
@@ -1133,7 +1121,7 @@
         <f aca="false">AH10*$AL$4</f>
         <v>20160</v>
       </c>
-      <c r="AM10" s="18" t="n">
+      <c r="AM10" s="15" t="n">
         <f aca="false">AJ10+5000</f>
         <v>17684</v>
       </c>
@@ -1151,7 +1139,7 @@
       <c r="E11" s="17" t="n">
         <v>3.3</v>
       </c>
-      <c r="F11" s="19" t="n">
+      <c r="F11" s="18" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="5" t="n">
@@ -1243,7 +1231,7 @@
       </c>
       <c r="AJ11" s="15"/>
       <c r="AK11" s="15"/>
-      <c r="AM11" s="18"/>
+      <c r="AM11" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
@@ -1258,10 +1246,10 @@
       <c r="D13" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E13" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="20" t="n">
+      <c r="E13" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="19" t="n">
         <v>0</v>
       </c>
       <c r="G13" s="10" t="n">
@@ -1361,7 +1349,7 @@
         <f aca="false">AH13*$AL$4</f>
         <v>21120</v>
       </c>
-      <c r="AM13" s="18" t="n">
+      <c r="AM13" s="15" t="n">
         <f aca="false">AJ13+5000</f>
         <v>15200</v>
       </c>
@@ -1376,10 +1364,10 @@
       <c r="D14" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="20" t="n">
+      <c r="E14" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19" t="n">
         <v>0</v>
       </c>
       <c r="G14" s="10" t="n">
@@ -1473,7 +1461,7 @@
       </c>
       <c r="AJ14" s="15"/>
       <c r="AK14" s="15"/>
-      <c r="AM14" s="18"/>
+      <c r="AM14" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
@@ -1509,16 +1497,16 @@
       <c r="K16" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="L16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="M16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="N16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="O16" s="21" t="n">
+      <c r="L16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="M16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="N16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="O16" s="10" t="n">
         <v>8</v>
       </c>
       <c r="P16" s="5" t="n">
@@ -1527,19 +1515,19 @@
       <c r="Q16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="R16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="S16" s="22" t="n">
-        <v>8</v>
-      </c>
-      <c r="T16" s="22" t="n">
-        <v>8</v>
-      </c>
-      <c r="U16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="V16" s="21" t="n">
+      <c r="R16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="S16" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="T16" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="U16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="V16" s="10" t="n">
         <v>8</v>
       </c>
       <c r="W16" s="5" t="n">
@@ -1548,19 +1536,19 @@
       <c r="X16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z16" s="22" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA16" s="22" t="n">
-        <v>8</v>
-      </c>
-      <c r="AB16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="AC16" s="21" t="n">
+      <c r="Y16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z16" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA16" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC16" s="10" t="n">
         <v>8</v>
       </c>
       <c r="AD16" s="5" t="n">
@@ -1569,10 +1557,10 @@
       <c r="AE16" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AF16" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="AG16" s="21" t="n">
+      <c r="AF16" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AG16" s="10" t="n">
         <v>8</v>
       </c>
       <c r="AH16" s="13" t="n">
@@ -1581,19 +1569,19 @@
       </c>
       <c r="AI16" s="14" t="n">
         <f aca="false">(AH16-AH17)</f>
-        <v>78.5</v>
+        <v>70.5</v>
       </c>
       <c r="AJ16" s="15" t="n">
         <f aca="false">(AH17*$AL$4)</f>
-        <v>6900</v>
+        <v>7860</v>
       </c>
       <c r="AK16" s="15" t="n">
         <f aca="false">AH16*$AL$4</f>
         <v>16320</v>
       </c>
-      <c r="AM16" s="18" t="n">
+      <c r="AM16" s="15" t="n">
         <f aca="false">AJ16+5000</f>
-        <v>11900</v>
+        <v>12860</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1624,19 +1612,19 @@
       <c r="J17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="K17" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="L17" s="21" t="n">
+      <c r="K17" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="L17" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="M17" s="21" t="n">
+      <c r="M17" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="N17" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="O17" s="21" t="n">
+      <c r="N17" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="O17" s="10" t="n">
         <v>8</v>
       </c>
       <c r="P17" s="5" t="n">
@@ -1645,19 +1633,19 @@
       <c r="Q17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="R17" s="21" t="n">
+      <c r="R17" s="10" t="n">
         <v>6.5</v>
       </c>
-      <c r="S17" s="21" t="n">
+      <c r="S17" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="T17" s="21" t="n">
-        <v>8</v>
-      </c>
-      <c r="U17" s="21" t="n">
+      <c r="T17" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="U17" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="V17" s="21" t="n">
+      <c r="V17" s="10" t="n">
         <v>0</v>
       </c>
       <c r="W17" s="5" t="n">
@@ -1666,19 +1654,19 @@
       <c r="X17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="Y17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="21" t="n">
+      <c r="Y17" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z17" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="10" t="n">
         <v>0</v>
       </c>
       <c r="AD17" s="5" t="n">
@@ -1687,23 +1675,23 @@
       <c r="AE17" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AF17" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="21" t="n">
+      <c r="AF17" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="10" t="n">
         <v>0</v>
       </c>
       <c r="AH17" s="13" t="n">
         <f aca="false">SUM($C17:$AG17)</f>
-        <v>57.5</v>
+        <v>65.5</v>
       </c>
       <c r="AI17" s="14" t="n">
         <f aca="false">(AI16*$AL$4)</f>
-        <v>9420</v>
+        <v>8460</v>
       </c>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>
-      <c r="AM17" s="18"/>
+      <c r="AM17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>

<commit_message>
new data - 23.01.2023 17:25:34,01
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y18" activeCellId="0" sqref="Y18"/>
+      <selection pane="topLeft" activeCell="Z17" activeCellId="0" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,11 +1569,11 @@
       </c>
       <c r="AI16" s="14" t="n">
         <f aca="false">(AH16-AH17)</f>
-        <v>70.5</v>
+        <v>69.5</v>
       </c>
       <c r="AJ16" s="15" t="n">
         <f aca="false">(AH17*$AL$4)</f>
-        <v>7860</v>
+        <v>7980</v>
       </c>
       <c r="AK16" s="15" t="n">
         <f aca="false">AH16*$AL$4</f>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="AM16" s="15" t="n">
         <f aca="false">AJ16+5000</f>
-        <v>12860</v>
+        <v>12980</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,7 +1658,7 @@
         <v>8</v>
       </c>
       <c r="Z17" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17" s="10" t="n">
         <v>0</v>
@@ -1683,11 +1683,11 @@
       </c>
       <c r="AH17" s="13" t="n">
         <f aca="false">SUM($C17:$AG17)</f>
-        <v>65.5</v>
+        <v>66.5</v>
       </c>
       <c r="AI17" s="14" t="n">
         <f aca="false">(AI16*$AL$4)</f>
-        <v>8460</v>
+        <v>8340</v>
       </c>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>

</xml_diff>

<commit_message>
new data - 23.01.2023 17:27:30,54
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z17" activeCellId="0" sqref="Z17"/>
+      <selection pane="topLeft" activeCell="Z18" activeCellId="0" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,11 +1569,11 @@
       </c>
       <c r="AI16" s="14" t="n">
         <f aca="false">(AH16-AH17)</f>
-        <v>69.5</v>
+        <v>70.5</v>
       </c>
       <c r="AJ16" s="15" t="n">
         <f aca="false">(AH17*$AL$4)</f>
-        <v>7980</v>
+        <v>7860</v>
       </c>
       <c r="AK16" s="15" t="n">
         <f aca="false">AH16*$AL$4</f>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="AM16" s="15" t="n">
         <f aca="false">AJ16+5000</f>
-        <v>12980</v>
+        <v>12860</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,7 +1658,7 @@
         <v>8</v>
       </c>
       <c r="Z17" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="10" t="n">
         <v>0</v>
@@ -1683,11 +1683,11 @@
       </c>
       <c r="AH17" s="13" t="n">
         <f aca="false">SUM($C17:$AG17)</f>
-        <v>66.5</v>
+        <v>65.5</v>
       </c>
       <c r="AI17" s="14" t="n">
         <f aca="false">(AI16*$AL$4)</f>
-        <v>8340</v>
+        <v>8460</v>
       </c>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>

</xml_diff>

<commit_message>
new data - 23.01.2023 17:28:02,92
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z18" activeCellId="0" sqref="Z18"/>
+      <selection pane="topLeft" activeCell="Z17" activeCellId="0" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,11 +1569,11 @@
       </c>
       <c r="AI16" s="14" t="n">
         <f aca="false">(AH16-AH17)</f>
-        <v>70.5</v>
+        <v>69.5</v>
       </c>
       <c r="AJ16" s="15" t="n">
         <f aca="false">(AH17*$AL$4)</f>
-        <v>7860</v>
+        <v>7980</v>
       </c>
       <c r="AK16" s="15" t="n">
         <f aca="false">AH16*$AL$4</f>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="AM16" s="15" t="n">
         <f aca="false">AJ16+5000</f>
-        <v>12860</v>
+        <v>12980</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,7 +1658,7 @@
         <v>8</v>
       </c>
       <c r="Z17" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17" s="10" t="n">
         <v>0</v>
@@ -1683,11 +1683,11 @@
       </c>
       <c r="AH17" s="13" t="n">
         <f aca="false">SUM($C17:$AG17)</f>
-        <v>65.5</v>
+        <v>66.5</v>
       </c>
       <c r="AI17" s="14" t="n">
         <f aca="false">(AI16*$AL$4)</f>
-        <v>8460</v>
+        <v>8340</v>
       </c>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>

</xml_diff>

<commit_message>
new data - 23.01.2023 17:29:00,73
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -375,7 +375,7 @@
   <dimension ref="A1:AM17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z17" activeCellId="0" sqref="Z17"/>
+      <selection pane="topLeft" activeCell="Z18" activeCellId="0" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1569,11 +1569,11 @@
       </c>
       <c r="AI16" s="14" t="n">
         <f aca="false">(AH16-AH17)</f>
-        <v>69.5</v>
+        <v>70.5</v>
       </c>
       <c r="AJ16" s="15" t="n">
         <f aca="false">(AH17*$AL$4)</f>
-        <v>7980</v>
+        <v>7860</v>
       </c>
       <c r="AK16" s="15" t="n">
         <f aca="false">AH16*$AL$4</f>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="AM16" s="15" t="n">
         <f aca="false">AJ16+5000</f>
-        <v>12980</v>
+        <v>12860</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,7 +1658,7 @@
         <v>8</v>
       </c>
       <c r="Z17" s="10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17" s="10" t="n">
         <v>0</v>
@@ -1683,11 +1683,11 @@
       </c>
       <c r="AH17" s="13" t="n">
         <f aca="false">SUM($C17:$AG17)</f>
-        <v>66.5</v>
+        <v>65.5</v>
       </c>
       <c r="AI17" s="14" t="n">
         <f aca="false">(AI16*$AL$4)</f>
-        <v>8340</v>
+        <v>8460</v>
       </c>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>

</xml_diff>

<commit_message>
new data - 26.01.2023 18:14:50,20
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilyab\Desktop\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAB9158-915C-4F52-8DE8-650B6E59C1CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E2773A-D67D-48F2-A5E0-4E04F49E758B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,10 +242,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,7 +633,7 @@
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AB18" sqref="AB18"/>
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,41 +652,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -915,11 +915,11 @@
         <f>(AH4-AH5)</f>
         <v>58.749999999999986</v>
       </c>
-      <c r="AJ4" s="19">
+      <c r="AJ4" s="18">
         <f>(AH5*$AL4)</f>
         <v>14070.000000000002</v>
       </c>
-      <c r="AK4" s="19">
+      <c r="AK4" s="18">
         <f>AH4*$AL4</f>
         <v>21120</v>
       </c>
@@ -1032,8 +1032,8 @@
         <f>(AI4*$AL4)</f>
         <v>7049.9999999999982</v>
       </c>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1143,15 +1143,15 @@
         <f>(AH7-AH8)</f>
         <v>58.7</v>
       </c>
-      <c r="AJ7" s="19">
+      <c r="AJ7" s="18">
         <f>(AH8*$AL4)</f>
         <v>13116</v>
       </c>
-      <c r="AK7" s="19">
+      <c r="AK7" s="18">
         <f>AH7*$AL4</f>
         <v>20160</v>
       </c>
-      <c r="AM7" s="19">
+      <c r="AM7" s="18">
         <f>AJ7+5000</f>
         <v>18116</v>
       </c>
@@ -1261,9 +1261,9 @@
         <f>(AI7*$AL4)</f>
         <v>7044</v>
       </c>
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-      <c r="AM8" s="19"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AM8" s="18"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1371,15 +1371,15 @@
         <f>(AH10-AH11)</f>
         <v>62.300000000000011</v>
       </c>
-      <c r="AJ10" s="19">
+      <c r="AJ10" s="18">
         <f>(AH11*AL4)</f>
         <v>12683.999999999998</v>
       </c>
-      <c r="AK10" s="19">
+      <c r="AK10" s="18">
         <f>AH10*$AL$4</f>
         <v>20160</v>
       </c>
-      <c r="AM10" s="19">
+      <c r="AM10" s="18">
         <f>AJ10+5000</f>
         <v>17684</v>
       </c>
@@ -1487,9 +1487,9 @@
         <f>(AI10*$AL4)</f>
         <v>7476.0000000000018</v>
       </c>
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-      <c r="AM11" s="19"/>
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+      <c r="AM11" s="18"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1599,15 +1599,15 @@
         <f>(AH13-AH14)</f>
         <v>91</v>
       </c>
-      <c r="AJ13" s="19">
+      <c r="AJ13" s="18">
         <f>(AH14*$AL$4)</f>
         <v>10200</v>
       </c>
-      <c r="AK13" s="19">
+      <c r="AK13" s="18">
         <f>AH13*$AL$4</f>
         <v>21120</v>
       </c>
-      <c r="AM13" s="19">
+      <c r="AM13" s="18">
         <f>AJ13+5000</f>
         <v>15200</v>
       </c>
@@ -1717,9 +1717,9 @@
         <f>(AI13*$AL$4)</f>
         <v>10920</v>
       </c>
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-      <c r="AM14" s="19"/>
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+      <c r="AM14" s="18"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1827,19 +1827,19 @@
       </c>
       <c r="AI16" s="13">
         <f>(AH16-AH17)</f>
-        <v>54.5</v>
-      </c>
-      <c r="AJ16" s="19">
+        <v>49.5</v>
+      </c>
+      <c r="AJ16" s="18">
         <f>(AH17*$AL$4)</f>
-        <v>9780</v>
-      </c>
-      <c r="AK16" s="19">
+        <v>10380</v>
+      </c>
+      <c r="AK16" s="18">
         <f>AH16*$AL$4</f>
         <v>16320</v>
       </c>
-      <c r="AM16" s="19">
+      <c r="AM16" s="18">
         <f>AJ16+5000</f>
-        <v>14780</v>
+        <v>15380</v>
       </c>
     </row>
     <row r="17" spans="2:39" x14ac:dyDescent="0.25">
@@ -1922,7 +1922,7 @@
         <v>8</v>
       </c>
       <c r="AB17" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC17" s="9">
         <v>0</v>
@@ -1941,18 +1941,23 @@
       </c>
       <c r="AH17" s="12">
         <f>SUM($C17:$AG17)</f>
-        <v>81.5</v>
+        <v>86.5</v>
       </c>
       <c r="AI17" s="13">
         <f>(AI16*$AL$4)</f>
-        <v>6540</v>
-      </c>
-      <c r="AJ17" s="19"/>
-      <c r="AK17" s="19"/>
-      <c r="AM17" s="19"/>
+        <v>5940</v>
+      </c>
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+      <c r="AM17" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AJ7:AJ8"/>
+    <mergeCell ref="AK7:AK8"/>
     <mergeCell ref="AJ16:AJ17"/>
     <mergeCell ref="AK16:AK17"/>
     <mergeCell ref="AM16:AM17"/>
@@ -1963,11 +1968,6 @@
     <mergeCell ref="AJ13:AJ14"/>
     <mergeCell ref="AK13:AK14"/>
     <mergeCell ref="AM13:AM14"/>
-    <mergeCell ref="A1:AG1"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AJ7:AJ8"/>
-    <mergeCell ref="AK7:AK8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
new data - 30.01.2023 17:21:21,34
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilyab\Desktop\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E2773A-D67D-48F2-A5E0-4E04F49E758B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E40051D-2BA8-4A43-912B-F6FA39153563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Парақ1" sheetId="1" r:id="rId1"/>
@@ -242,10 +242,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -632,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,41 +652,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="19"/>
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -915,11 +915,11 @@
         <f>(AH4-AH5)</f>
         <v>58.749999999999986</v>
       </c>
-      <c r="AJ4" s="18">
+      <c r="AJ4" s="19">
         <f>(AH5*$AL4)</f>
         <v>14070.000000000002</v>
       </c>
-      <c r="AK4" s="18">
+      <c r="AK4" s="19">
         <f>AH4*$AL4</f>
         <v>21120</v>
       </c>
@@ -1032,8 +1032,8 @@
         <f>(AI4*$AL4)</f>
         <v>7049.9999999999982</v>
       </c>
-      <c r="AJ5" s="18"/>
-      <c r="AK5" s="18"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1143,15 +1143,15 @@
         <f>(AH7-AH8)</f>
         <v>58.7</v>
       </c>
-      <c r="AJ7" s="18">
+      <c r="AJ7" s="19">
         <f>(AH8*$AL4)</f>
         <v>13116</v>
       </c>
-      <c r="AK7" s="18">
+      <c r="AK7" s="19">
         <f>AH7*$AL4</f>
         <v>20160</v>
       </c>
-      <c r="AM7" s="18">
+      <c r="AM7" s="19">
         <f>AJ7+5000</f>
         <v>18116</v>
       </c>
@@ -1261,9 +1261,9 @@
         <f>(AI7*$AL4)</f>
         <v>7044</v>
       </c>
-      <c r="AJ8" s="18"/>
-      <c r="AK8" s="18"/>
-      <c r="AM8" s="18"/>
+      <c r="AJ8" s="19"/>
+      <c r="AK8" s="19"/>
+      <c r="AM8" s="19"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1371,15 +1371,15 @@
         <f>(AH10-AH11)</f>
         <v>62.300000000000011</v>
       </c>
-      <c r="AJ10" s="18">
+      <c r="AJ10" s="19">
         <f>(AH11*AL4)</f>
         <v>12683.999999999998</v>
       </c>
-      <c r="AK10" s="18">
+      <c r="AK10" s="19">
         <f>AH10*$AL$4</f>
         <v>20160</v>
       </c>
-      <c r="AM10" s="18">
+      <c r="AM10" s="19">
         <f>AJ10+5000</f>
         <v>17684</v>
       </c>
@@ -1487,9 +1487,9 @@
         <f>(AI10*$AL4)</f>
         <v>7476.0000000000018</v>
       </c>
-      <c r="AJ11" s="18"/>
-      <c r="AK11" s="18"/>
-      <c r="AM11" s="18"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AM11" s="19"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1599,15 +1599,15 @@
         <f>(AH13-AH14)</f>
         <v>91</v>
       </c>
-      <c r="AJ13" s="18">
+      <c r="AJ13" s="19">
         <f>(AH14*$AL$4)</f>
         <v>10200</v>
       </c>
-      <c r="AK13" s="18">
+      <c r="AK13" s="19">
         <f>AH13*$AL$4</f>
         <v>21120</v>
       </c>
-      <c r="AM13" s="18">
+      <c r="AM13" s="19">
         <f>AJ13+5000</f>
         <v>15200</v>
       </c>
@@ -1717,9 +1717,9 @@
         <f>(AI13*$AL$4)</f>
         <v>10920</v>
       </c>
-      <c r="AJ14" s="18"/>
-      <c r="AK14" s="18"/>
-      <c r="AM14" s="18"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
+      <c r="AM14" s="19"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1827,19 +1827,19 @@
       </c>
       <c r="AI16" s="13">
         <f>(AH16-AH17)</f>
-        <v>49.5</v>
-      </c>
-      <c r="AJ16" s="18">
+        <v>41.5</v>
+      </c>
+      <c r="AJ16" s="19">
         <f>(AH17*$AL$4)</f>
-        <v>10380</v>
-      </c>
-      <c r="AK16" s="18">
+        <v>11340</v>
+      </c>
+      <c r="AK16" s="19">
         <f>AH16*$AL$4</f>
         <v>16320</v>
       </c>
-      <c r="AM16" s="18">
+      <c r="AM16" s="19">
         <f>AJ16+5000</f>
-        <v>15380</v>
+        <v>16340</v>
       </c>
     </row>
     <row r="17" spans="2:39" x14ac:dyDescent="0.25">
@@ -1934,30 +1934,25 @@
         <v>0</v>
       </c>
       <c r="AF17" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG17" s="9">
         <v>0</v>
       </c>
       <c r="AH17" s="12">
         <f>SUM($C17:$AG17)</f>
-        <v>86.5</v>
+        <v>94.5</v>
       </c>
       <c r="AI17" s="13">
         <f>(AI16*$AL$4)</f>
-        <v>5940</v>
-      </c>
-      <c r="AJ17" s="18"/>
-      <c r="AK17" s="18"/>
-      <c r="AM17" s="18"/>
+        <v>4980</v>
+      </c>
+      <c r="AJ17" s="19"/>
+      <c r="AK17" s="19"/>
+      <c r="AM17" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:AG1"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AJ7:AJ8"/>
-    <mergeCell ref="AK7:AK8"/>
     <mergeCell ref="AJ16:AJ17"/>
     <mergeCell ref="AK16:AK17"/>
     <mergeCell ref="AM16:AM17"/>
@@ -1968,6 +1963,11 @@
     <mergeCell ref="AJ13:AJ14"/>
     <mergeCell ref="AK13:AK14"/>
     <mergeCell ref="AM13:AM14"/>
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AJ7:AJ8"/>
+    <mergeCell ref="AK7:AK8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
new data - 31.01.2023 17:38:27,04
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilyab\Desktop\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E40051D-2BA8-4A43-912B-F6FA39153563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56F26E6-324B-4650-AFED-990BE58EBC97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,10 +242,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,7 +633,7 @@
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5"/>
+      <selection activeCell="AI25" sqref="AI25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,41 +652,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -915,11 +915,11 @@
         <f>(AH4-AH5)</f>
         <v>58.749999999999986</v>
       </c>
-      <c r="AJ4" s="19">
+      <c r="AJ4" s="18">
         <f>(AH5*$AL4)</f>
         <v>14070.000000000002</v>
       </c>
-      <c r="AK4" s="19">
+      <c r="AK4" s="18">
         <f>AH4*$AL4</f>
         <v>21120</v>
       </c>
@@ -1032,8 +1032,8 @@
         <f>(AI4*$AL4)</f>
         <v>7049.9999999999982</v>
       </c>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1143,15 +1143,15 @@
         <f>(AH7-AH8)</f>
         <v>58.7</v>
       </c>
-      <c r="AJ7" s="19">
+      <c r="AJ7" s="18">
         <f>(AH8*$AL4)</f>
         <v>13116</v>
       </c>
-      <c r="AK7" s="19">
+      <c r="AK7" s="18">
         <f>AH7*$AL4</f>
         <v>20160</v>
       </c>
-      <c r="AM7" s="19">
+      <c r="AM7" s="18">
         <f>AJ7+5000</f>
         <v>18116</v>
       </c>
@@ -1261,9 +1261,9 @@
         <f>(AI7*$AL4)</f>
         <v>7044</v>
       </c>
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-      <c r="AM8" s="19"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AM8" s="18"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1371,15 +1371,15 @@
         <f>(AH10-AH11)</f>
         <v>62.300000000000011</v>
       </c>
-      <c r="AJ10" s="19">
+      <c r="AJ10" s="18">
         <f>(AH11*AL4)</f>
         <v>12683.999999999998</v>
       </c>
-      <c r="AK10" s="19">
+      <c r="AK10" s="18">
         <f>AH10*$AL$4</f>
         <v>20160</v>
       </c>
-      <c r="AM10" s="19">
+      <c r="AM10" s="18">
         <f>AJ10+5000</f>
         <v>17684</v>
       </c>
@@ -1487,9 +1487,9 @@
         <f>(AI10*$AL4)</f>
         <v>7476.0000000000018</v>
       </c>
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-      <c r="AM11" s="19"/>
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+      <c r="AM11" s="18"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1599,15 +1599,15 @@
         <f>(AH13-AH14)</f>
         <v>91</v>
       </c>
-      <c r="AJ13" s="19">
+      <c r="AJ13" s="18">
         <f>(AH14*$AL$4)</f>
         <v>10200</v>
       </c>
-      <c r="AK13" s="19">
+      <c r="AK13" s="18">
         <f>AH13*$AL$4</f>
         <v>21120</v>
       </c>
-      <c r="AM13" s="19">
+      <c r="AM13" s="18">
         <f>AJ13+5000</f>
         <v>15200</v>
       </c>
@@ -1717,9 +1717,9 @@
         <f>(AI13*$AL$4)</f>
         <v>10920</v>
       </c>
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-      <c r="AM14" s="19"/>
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+      <c r="AM14" s="18"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1827,19 +1827,19 @@
       </c>
       <c r="AI16" s="13">
         <f>(AH16-AH17)</f>
-        <v>41.5</v>
-      </c>
-      <c r="AJ16" s="19">
+        <v>33.5</v>
+      </c>
+      <c r="AJ16" s="18">
         <f>(AH17*$AL$4)</f>
-        <v>11340</v>
-      </c>
-      <c r="AK16" s="19">
+        <v>12300</v>
+      </c>
+      <c r="AK16" s="18">
         <f>AH16*$AL$4</f>
         <v>16320</v>
       </c>
-      <c r="AM16" s="19">
+      <c r="AM16" s="18">
         <f>AJ16+5000</f>
-        <v>16340</v>
+        <v>17300</v>
       </c>
     </row>
     <row r="17" spans="2:39" x14ac:dyDescent="0.25">
@@ -1937,22 +1937,27 @@
         <v>8</v>
       </c>
       <c r="AG17" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AH17" s="12">
         <f>SUM($C17:$AG17)</f>
-        <v>94.5</v>
+        <v>102.5</v>
       </c>
       <c r="AI17" s="13">
         <f>(AI16*$AL$4)</f>
-        <v>4980</v>
-      </c>
-      <c r="AJ17" s="19"/>
-      <c r="AK17" s="19"/>
-      <c r="AM17" s="19"/>
+        <v>4020</v>
+      </c>
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+      <c r="AM17" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AJ7:AJ8"/>
+    <mergeCell ref="AK7:AK8"/>
     <mergeCell ref="AJ16:AJ17"/>
     <mergeCell ref="AK16:AK17"/>
     <mergeCell ref="AM16:AM17"/>
@@ -1963,11 +1968,6 @@
     <mergeCell ref="AJ13:AJ14"/>
     <mergeCell ref="AK13:AK14"/>
     <mergeCell ref="AM13:AM14"/>
-    <mergeCell ref="A1:AG1"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AJ7:AJ8"/>
-    <mergeCell ref="AK7:AK8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
new data - 02.02.2023 18:36:59,89
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -217,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,15 +298,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,7 +382,7 @@
   <dimension ref="A1:AM20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X28" activeCellId="0" sqref="X28"/>
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -400,10 +392,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="3" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="21.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="40" style="1" width="9"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="1" width="11.86"/>
   </cols>
@@ -1418,7 +1410,7 @@
       <c r="Q14" s="10" t="n">
         <v>3.5</v>
       </c>
-      <c r="R14" s="20" t="n">
+      <c r="R14" s="10" t="n">
         <v>6</v>
       </c>
       <c r="S14" s="11" t="n">
@@ -1715,13 +1707,13 @@
       <c r="B19" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="D19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="E19" s="21" t="n">
+      <c r="C19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E19" s="20" t="n">
         <v>8</v>
       </c>
       <c r="F19" s="19" t="n">
@@ -1730,19 +1722,19 @@
       <c r="G19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="I19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="J19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="K19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="L19" s="20" t="n">
+      <c r="H19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="I19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="K19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="L19" s="10" t="n">
         <v>8</v>
       </c>
       <c r="M19" s="5" t="n">
@@ -1751,19 +1743,19 @@
       <c r="N19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="O19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="P19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="R19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="S19" s="22" t="n">
+      <c r="O19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="P19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="R19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="S19" s="17" t="n">
         <v>8</v>
       </c>
       <c r="T19" s="11" t="n">
@@ -1772,19 +1764,19 @@
       <c r="U19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="W19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="X19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="Y19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z19" s="22" t="n">
+      <c r="V19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="W19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="X19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z19" s="17" t="n">
         <v>8</v>
       </c>
       <c r="AA19" s="11" t="n">
@@ -1793,26 +1785,26 @@
       <c r="AB19" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AC19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="AD19" s="20" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE19" s="20"/>
-      <c r="AF19" s="20"/>
-      <c r="AG19" s="20"/>
+      <c r="AC19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD19" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
       <c r="AH19" s="13" t="n">
         <f aca="false">SUM($C19:$AG19)</f>
         <v>160</v>
       </c>
       <c r="AI19" s="14" t="n">
         <f aca="false">(AH19-AH20)</f>
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="AJ19" s="15" t="n">
         <f aca="false">(AH20*$AL$4)</f>
-        <v>0</v>
+        <v>1920</v>
       </c>
       <c r="AK19" s="15" t="n">
         <f aca="false">AH19*$AL$4</f>
@@ -1820,67 +1812,71 @@
       </c>
       <c r="AM19" s="15" t="n">
         <f aca="false">AJ19+5000</f>
-        <v>5000</v>
+        <v>6920</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
+      <c r="C20" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D20" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" s="20"/>
       <c r="F20" s="19" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
       <c r="M20" s="5" t="n">
         <v>0</v>
       </c>
       <c r="N20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="22"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="17"/>
       <c r="T20" s="11" t="n">
         <v>0</v>
       </c>
       <c r="U20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="V20" s="20"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="20"/>
-      <c r="Y20" s="20"/>
-      <c r="Z20" s="22"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="17"/>
       <c r="AA20" s="11" t="n">
         <v>0</v>
       </c>
       <c r="AB20" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AC20" s="20"/>
-      <c r="AD20" s="20"/>
-      <c r="AE20" s="20"/>
-      <c r="AF20" s="20"/>
-      <c r="AG20" s="20"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
       <c r="AH20" s="13" t="n">
         <f aca="false">SUM($C20:$AG20)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AI20" s="14" t="n">
         <f aca="false">(AI19*$AL$4)</f>
-        <v>19200</v>
+        <v>17280</v>
       </c>
       <c r="AJ20" s="15"/>
       <c r="AK20" s="15"/>

</xml_diff>

<commit_message>
new data - 14.02.2023 12:21:25,83
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilyab\Desktop\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F6D8A5-555D-4376-A86B-FF8F0209672A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657EBDCB-9A8E-43D7-A299-D9BF892FF843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +164,12 @@
         <bgColor rgb="FFFF3838"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -192,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,10 +254,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -639,7 +648,7 @@
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,41 +667,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19"/>
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -921,11 +930,11 @@
         <f>(AH4-AH5)</f>
         <v>58.749999999999986</v>
       </c>
-      <c r="AJ4" s="19">
+      <c r="AJ4" s="20">
         <f>(AH5*$AL4)</f>
         <v>14070.000000000002</v>
       </c>
-      <c r="AK4" s="19">
+      <c r="AK4" s="20">
         <f>AH4*$AL4</f>
         <v>21120</v>
       </c>
@@ -1038,8 +1047,8 @@
         <f>(AI4*$AL4)</f>
         <v>7049.9999999999982</v>
       </c>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1149,15 +1158,15 @@
         <f>(AH7-AH8)</f>
         <v>58.7</v>
       </c>
-      <c r="AJ7" s="19">
+      <c r="AJ7" s="20">
         <f>(AH8*$AL4)</f>
         <v>13116</v>
       </c>
-      <c r="AK7" s="19">
+      <c r="AK7" s="20">
         <f>AH7*$AL4</f>
         <v>20160</v>
       </c>
-      <c r="AM7" s="19">
+      <c r="AM7" s="20">
         <f>AJ7+5000</f>
         <v>18116</v>
       </c>
@@ -1267,9 +1276,9 @@
         <f>(AI7*$AL4)</f>
         <v>7044</v>
       </c>
-      <c r="AJ8" s="19"/>
-      <c r="AK8" s="19"/>
-      <c r="AM8" s="19"/>
+      <c r="AJ8" s="20"/>
+      <c r="AK8" s="20"/>
+      <c r="AM8" s="20"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1377,15 +1386,15 @@
         <f>(AH10-AH11)</f>
         <v>62.300000000000011</v>
       </c>
-      <c r="AJ10" s="19">
+      <c r="AJ10" s="20">
         <f>(AH11*AL4)</f>
         <v>12683.999999999998</v>
       </c>
-      <c r="AK10" s="19">
+      <c r="AK10" s="20">
         <f>AH10*$AL$4</f>
         <v>20160</v>
       </c>
-      <c r="AM10" s="19">
+      <c r="AM10" s="20">
         <f>AJ10+5000</f>
         <v>17684</v>
       </c>
@@ -1493,9 +1502,9 @@
         <f>(AI10*$AL4)</f>
         <v>7476.0000000000018</v>
       </c>
-      <c r="AJ11" s="19"/>
-      <c r="AK11" s="19"/>
-      <c r="AM11" s="19"/>
+      <c r="AJ11" s="20"/>
+      <c r="AK11" s="20"/>
+      <c r="AM11" s="20"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1605,15 +1614,15 @@
         <f>(AH13-AH14)</f>
         <v>91</v>
       </c>
-      <c r="AJ13" s="19">
+      <c r="AJ13" s="20">
         <f>(AH14*$AL$4)</f>
         <v>10200</v>
       </c>
-      <c r="AK13" s="19">
+      <c r="AK13" s="20">
         <f>AH13*$AL$4</f>
         <v>21120</v>
       </c>
-      <c r="AM13" s="19">
+      <c r="AM13" s="20">
         <f>AJ13+5000</f>
         <v>15200</v>
       </c>
@@ -1723,9 +1732,9 @@
         <f>(AI13*$AL$4)</f>
         <v>10920</v>
       </c>
-      <c r="AJ14" s="19"/>
-      <c r="AK14" s="19"/>
-      <c r="AM14" s="19"/>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="20"/>
+      <c r="AM14" s="20"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1835,15 +1844,15 @@
         <f>(AH16-AH17)</f>
         <v>33.5</v>
       </c>
-      <c r="AJ16" s="19">
+      <c r="AJ16" s="20">
         <f>(AH17*$AL$4)</f>
         <v>12300</v>
       </c>
-      <c r="AK16" s="19">
+      <c r="AK16" s="20">
         <f>AH16*$AL$4</f>
         <v>16320</v>
       </c>
-      <c r="AM16" s="19">
+      <c r="AM16" s="20">
         <f>AJ16+5000</f>
         <v>17300</v>
       </c>
@@ -1953,9 +1962,9 @@
         <f>(AI16*$AL$4)</f>
         <v>4020</v>
       </c>
-      <c r="AJ17" s="19"/>
-      <c r="AK17" s="19"/>
-      <c r="AM17" s="19"/>
+      <c r="AJ17" s="20"/>
+      <c r="AK17" s="20"/>
+      <c r="AM17" s="20"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -2057,19 +2066,19 @@
       </c>
       <c r="AI19" s="13">
         <f>(AH19-AH20)</f>
-        <v>136</v>
-      </c>
-      <c r="AJ19" s="19">
+        <v>116</v>
+      </c>
+      <c r="AJ19" s="20">
         <f>(AH20*$AL$4)</f>
-        <v>2880</v>
-      </c>
-      <c r="AK19" s="19">
+        <v>5280</v>
+      </c>
+      <c r="AK19" s="20">
         <f>AH19*$AL$4</f>
         <v>19200</v>
       </c>
-      <c r="AM19" s="19">
+      <c r="AM19" s="20">
         <f>AJ19+5000</f>
-        <v>7880</v>
+        <v>10280</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
@@ -2091,11 +2100,21 @@
       <c r="G20" s="4">
         <v>0</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
+      <c r="H20" s="21">
+        <v>4</v>
+      </c>
+      <c r="I20" s="21">
+        <v>4</v>
+      </c>
+      <c r="J20" s="21">
+        <v>4</v>
+      </c>
+      <c r="K20" s="21">
+        <v>4</v>
+      </c>
+      <c r="L20" s="21">
+        <v>4</v>
+      </c>
       <c r="M20" s="4">
         <v>0</v>
       </c>
@@ -2131,23 +2150,24 @@
       <c r="AG20" s="9"/>
       <c r="AH20" s="12">
         <f>SUM($C20:$AG20)</f>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="AI20" s="13">
         <f>(AI19*$AL$4)</f>
-        <v>16320</v>
-      </c>
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-      <c r="AM20" s="19"/>
+        <v>13920</v>
+      </c>
+      <c r="AJ20" s="20"/>
+      <c r="AK20" s="20"/>
+      <c r="AM20" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:AG1"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AJ7:AJ8"/>
-    <mergeCell ref="AK7:AK8"/>
+    <mergeCell ref="AJ16:AJ17"/>
+    <mergeCell ref="AK16:AK17"/>
+    <mergeCell ref="AM16:AM17"/>
+    <mergeCell ref="AJ19:AJ20"/>
+    <mergeCell ref="AK19:AK20"/>
+    <mergeCell ref="AM19:AM20"/>
     <mergeCell ref="AM7:AM8"/>
     <mergeCell ref="AJ10:AJ11"/>
     <mergeCell ref="AK10:AK11"/>
@@ -2155,12 +2175,11 @@
     <mergeCell ref="AJ13:AJ14"/>
     <mergeCell ref="AK13:AK14"/>
     <mergeCell ref="AM13:AM14"/>
-    <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AK16:AK17"/>
-    <mergeCell ref="AM16:AM17"/>
-    <mergeCell ref="AJ19:AJ20"/>
-    <mergeCell ref="AK19:AK20"/>
-    <mergeCell ref="AM19:AM20"/>
+    <mergeCell ref="A1:AG1"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AJ7:AJ8"/>
+    <mergeCell ref="AK7:AK8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
new data - 21.02.2023 18:36:38,13
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -232,9 +232,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,22 +257,25 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE34" sqref="AE34"/>
+    <sheetView tabSelected="1" topLeftCell="O5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,162 +679,162 @@
     <col min="39" max="39" width="27.28515625" style="8" customWidth="1"/>
     <col min="40" max="64" width="9" style="8" customWidth="1"/>
     <col min="65" max="1024" width="11.85546875" style="8"/>
-    <col min="1025" max="16384" width="11.85546875" style="11"/>
+    <col min="1025" max="16384" width="11.85546875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="12">
         <v>1</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>2</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>3</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="12">
         <v>4</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="12">
         <v>5</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>6</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <v>7</v>
       </c>
-      <c r="J2" s="13">
-        <v>8</v>
-      </c>
-      <c r="K2" s="13">
+      <c r="J2" s="12">
+        <v>8</v>
+      </c>
+      <c r="K2" s="12">
         <v>9</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="12">
         <v>10</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="12">
         <v>11</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2" s="12">
         <v>12</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="12">
         <v>13</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="12">
         <v>14</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="12">
         <v>15</v>
       </c>
-      <c r="R2" s="13">
+      <c r="R2" s="12">
         <v>16</v>
       </c>
-      <c r="S2" s="13">
+      <c r="S2" s="12">
         <v>17</v>
       </c>
-      <c r="T2" s="13">
+      <c r="T2" s="12">
         <v>18</v>
       </c>
-      <c r="U2" s="13">
+      <c r="U2" s="12">
         <v>19</v>
       </c>
-      <c r="V2" s="13">
+      <c r="V2" s="12">
         <v>20</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="12">
         <v>21</v>
       </c>
-      <c r="X2" s="13">
+      <c r="X2" s="12">
         <v>22</v>
       </c>
-      <c r="Y2" s="13">
+      <c r="Y2" s="12">
         <v>23</v>
       </c>
-      <c r="Z2" s="13">
+      <c r="Z2" s="12">
         <v>24</v>
       </c>
-      <c r="AA2" s="13">
+      <c r="AA2" s="12">
         <v>25</v>
       </c>
-      <c r="AB2" s="13">
+      <c r="AB2" s="12">
         <v>26</v>
       </c>
-      <c r="AC2" s="13">
+      <c r="AC2" s="12">
         <v>27</v>
       </c>
-      <c r="AD2" s="13">
+      <c r="AD2" s="12">
         <v>28</v>
       </c>
-      <c r="AE2" s="13">
+      <c r="AE2" s="12">
         <v>29</v>
       </c>
-      <c r="AF2" s="13">
+      <c r="AF2" s="12">
         <v>30</v>
       </c>
-      <c r="AG2" s="13">
+      <c r="AG2" s="12">
         <v>31</v>
       </c>
-      <c r="AH2" s="13" t="s">
+      <c r="AH2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="AI2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="14" t="s">
+      <c r="AJ2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" s="15" t="s">
+      <c r="AK2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AM2" s="16" t="s">
+      <c r="AM2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -872,10 +872,10 @@
       <c r="K4" s="2">
         <v>8</v>
       </c>
-      <c r="L4" s="17">
-        <v>0</v>
-      </c>
-      <c r="M4" s="17">
+      <c r="L4" s="16">
+        <v>0</v>
+      </c>
+      <c r="M4" s="16">
         <v>0</v>
       </c>
       <c r="N4" s="2">
@@ -938,23 +938,23 @@
       <c r="AG4" s="5">
         <v>0</v>
       </c>
-      <c r="AH4" s="18">
+      <c r="AH4" s="17">
         <f>SUM($C4:$AG4)</f>
         <v>176</v>
       </c>
-      <c r="AI4" s="19">
+      <c r="AI4" s="18">
         <f>(AH4-AH5)</f>
         <v>58.749999999999986</v>
       </c>
-      <c r="AJ4" s="20">
+      <c r="AJ4" s="24">
         <f>(AH5*$AL4)</f>
         <v>14070.000000000002</v>
       </c>
-      <c r="AK4" s="20">
+      <c r="AK4" s="24">
         <f>AH4*$AL4</f>
         <v>21120</v>
       </c>
-      <c r="AL4" s="21">
+      <c r="AL4" s="19">
         <v>120</v>
       </c>
     </row>
@@ -989,10 +989,10 @@
       <c r="K5" s="2">
         <v>6.2</v>
       </c>
-      <c r="L5" s="17">
-        <v>0</v>
-      </c>
-      <c r="M5" s="17">
+      <c r="L5" s="16">
+        <v>0</v>
+      </c>
+      <c r="M5" s="16">
         <v>0</v>
       </c>
       <c r="N5" s="2">
@@ -1055,16 +1055,16 @@
       <c r="AG5" s="5">
         <v>0</v>
       </c>
-      <c r="AH5" s="18">
+      <c r="AH5" s="17">
         <f>SUM($C5:$AG5)</f>
         <v>117.25000000000001</v>
       </c>
-      <c r="AI5" s="19">
+      <c r="AI5" s="18">
         <f>(AI4*$AL4)</f>
         <v>7049.9999999999982</v>
       </c>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20"/>
+      <c r="AJ5" s="24"/>
+      <c r="AK5" s="24"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1166,23 +1166,23 @@
       <c r="AG7" s="2">
         <v>8</v>
       </c>
-      <c r="AH7" s="18">
+      <c r="AH7" s="17">
         <f>SUM($C7:$AG7)</f>
         <v>168</v>
       </c>
-      <c r="AI7" s="19">
+      <c r="AI7" s="18">
         <f>(AH7-AH8)</f>
         <v>58.7</v>
       </c>
-      <c r="AJ7" s="20">
+      <c r="AJ7" s="24">
         <f>(AH8*$AL4)</f>
         <v>13116</v>
       </c>
-      <c r="AK7" s="20">
+      <c r="AK7" s="24">
         <f>AH7*$AL4</f>
         <v>20160</v>
       </c>
-      <c r="AM7" s="20">
+      <c r="AM7" s="24">
         <f>AJ7+5000</f>
         <v>18116</v>
       </c>
@@ -1284,17 +1284,17 @@
       <c r="AG8" s="2">
         <v>5.5</v>
       </c>
-      <c r="AH8" s="18">
+      <c r="AH8" s="17">
         <f>SUM($C8:$AG8)</f>
         <v>109.3</v>
       </c>
-      <c r="AI8" s="19">
+      <c r="AI8" s="18">
         <f>(AI7*$AL4)</f>
         <v>7044</v>
       </c>
-      <c r="AJ8" s="20"/>
-      <c r="AK8" s="20"/>
-      <c r="AM8" s="20"/>
+      <c r="AJ8" s="24"/>
+      <c r="AK8" s="24"/>
+      <c r="AM8" s="24"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1312,7 +1312,7 @@
       <c r="E10" s="6">
         <v>8</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="20">
         <v>0</v>
       </c>
       <c r="G10" s="5">
@@ -1394,23 +1394,23 @@
         <v>8</v>
       </c>
       <c r="AG10" s="2"/>
-      <c r="AH10" s="18">
+      <c r="AH10" s="17">
         <f>SUM($C10:$AG10)</f>
         <v>168</v>
       </c>
-      <c r="AI10" s="19">
+      <c r="AI10" s="18">
         <f>(AH10-AH11)</f>
         <v>62.300000000000011</v>
       </c>
-      <c r="AJ10" s="20">
+      <c r="AJ10" s="24">
         <f>(AH11*AL4)</f>
         <v>12683.999999999998</v>
       </c>
-      <c r="AK10" s="20">
+      <c r="AK10" s="24">
         <f>AH10*$AL$4</f>
         <v>20160</v>
       </c>
-      <c r="AM10" s="20">
+      <c r="AM10" s="24">
         <f>AJ10+5000</f>
         <v>17684</v>
       </c>
@@ -1428,7 +1428,7 @@
       <c r="E11" s="6">
         <v>3.3</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="20">
         <v>0</v>
       </c>
       <c r="G11" s="5">
@@ -1510,17 +1510,17 @@
         <v>6</v>
       </c>
       <c r="AG11" s="2"/>
-      <c r="AH11" s="18">
+      <c r="AH11" s="17">
         <f>SUM($C11:$AG11)</f>
         <v>105.69999999999999</v>
       </c>
-      <c r="AI11" s="19">
+      <c r="AI11" s="18">
         <f>(AI10*$AL4)</f>
         <v>7476.0000000000018</v>
       </c>
-      <c r="AJ11" s="20"/>
-      <c r="AK11" s="20"/>
-      <c r="AM11" s="20"/>
+      <c r="AJ11" s="24"/>
+      <c r="AK11" s="24"/>
+      <c r="AM11" s="24"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1622,23 +1622,23 @@
       <c r="AG13" s="5">
         <v>0</v>
       </c>
-      <c r="AH13" s="18">
+      <c r="AH13" s="17">
         <f>SUM($C13:$AG13)</f>
         <v>176</v>
       </c>
-      <c r="AI13" s="19">
+      <c r="AI13" s="18">
         <f>(AH13-AH14)</f>
         <v>91</v>
       </c>
-      <c r="AJ13" s="20">
+      <c r="AJ13" s="24">
         <f>(AH14*$AL$4)</f>
         <v>10200</v>
       </c>
-      <c r="AK13" s="20">
+      <c r="AK13" s="24">
         <f>AH13*$AL$4</f>
         <v>21120</v>
       </c>
-      <c r="AM13" s="20">
+      <c r="AM13" s="24">
         <f>AJ13+5000</f>
         <v>15200</v>
       </c>
@@ -1740,17 +1740,17 @@
       <c r="AG14" s="5">
         <v>0</v>
       </c>
-      <c r="AH14" s="18">
+      <c r="AH14" s="17">
         <f>SUM($C14:$AG14)</f>
         <v>85</v>
       </c>
-      <c r="AI14" s="19">
+      <c r="AI14" s="18">
         <f>(AI13*$AL$4)</f>
         <v>10920</v>
       </c>
-      <c r="AJ14" s="20"/>
-      <c r="AK14" s="20"/>
-      <c r="AM14" s="20"/>
+      <c r="AJ14" s="24"/>
+      <c r="AK14" s="24"/>
+      <c r="AM14" s="24"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1852,23 +1852,23 @@
       <c r="AG16" s="2">
         <v>8</v>
       </c>
-      <c r="AH16" s="18">
+      <c r="AH16" s="17">
         <f>SUM($C16:$AG16)</f>
         <v>136</v>
       </c>
-      <c r="AI16" s="19">
+      <c r="AI16" s="18">
         <f>(AH16-AH17)</f>
         <v>33.5</v>
       </c>
-      <c r="AJ16" s="20">
+      <c r="AJ16" s="24">
         <f>(AH17*$AL$4)</f>
         <v>12300</v>
       </c>
-      <c r="AK16" s="20">
+      <c r="AK16" s="24">
         <f>AH16*$AL$4</f>
         <v>16320</v>
       </c>
-      <c r="AM16" s="20">
+      <c r="AM16" s="24">
         <f>AJ16+5000</f>
         <v>17300</v>
       </c>
@@ -1970,17 +1970,17 @@
       <c r="AG17" s="2">
         <v>8</v>
       </c>
-      <c r="AH17" s="18">
+      <c r="AH17" s="17">
         <f>SUM($C17:$AG17)</f>
         <v>102.5</v>
       </c>
-      <c r="AI17" s="19">
+      <c r="AI17" s="18">
         <f>(AI16*$AL$4)</f>
         <v>4020</v>
       </c>
-      <c r="AJ17" s="20"/>
-      <c r="AK17" s="20"/>
-      <c r="AM17" s="20"/>
+      <c r="AJ17" s="24"/>
+      <c r="AK17" s="24"/>
+      <c r="AM17" s="24"/>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -2055,10 +2055,10 @@
       <c r="X19" s="2">
         <v>8</v>
       </c>
-      <c r="Y19" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="25">
+      <c r="Y19" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="23">
         <v>0</v>
       </c>
       <c r="AA19" s="7">
@@ -2076,25 +2076,25 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="18">
+      <c r="AH19" s="17">
         <f>SUM($C19:$AG19)</f>
         <v>144</v>
       </c>
-      <c r="AI19" s="19">
+      <c r="AI19" s="18">
         <f>(AH19-AH20)</f>
-        <v>98.5</v>
-      </c>
-      <c r="AJ19" s="20">
+        <v>92</v>
+      </c>
+      <c r="AJ19" s="24">
         <f>(AH20*$AL$4)</f>
-        <v>5460</v>
-      </c>
-      <c r="AK19" s="20">
+        <v>6240</v>
+      </c>
+      <c r="AK19" s="24">
         <f>AH19*$AL$4</f>
         <v>17280</v>
       </c>
-      <c r="AM19" s="20">
+      <c r="AM19" s="24">
         <f>AJ19+5000</f>
-        <v>10460</v>
+        <v>11240</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
@@ -2159,14 +2159,16 @@
         <v>0</v>
       </c>
       <c r="V20" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="W20" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="W20" s="2">
+        <v>5</v>
+      </c>
       <c r="X20" s="2"/>
-      <c r="Y20" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="24">
+      <c r="Y20" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="22">
         <v>0</v>
       </c>
       <c r="AA20" s="7">
@@ -2180,17 +2182,17 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
-      <c r="AH20" s="18">
+      <c r="AH20" s="17">
         <f>SUM($C20:$AG20)</f>
-        <v>45.5</v>
-      </c>
-      <c r="AI20" s="19">
+        <v>52</v>
+      </c>
+      <c r="AI20" s="18">
         <f>(AI19*$AL$4)</f>
-        <v>11820</v>
-      </c>
-      <c r="AJ20" s="20"/>
-      <c r="AK20" s="20"/>
-      <c r="AM20" s="20"/>
+        <v>11040</v>
+      </c>
+      <c r="AJ20" s="24"/>
+      <c r="AK20" s="24"/>
+      <c r="AM20" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="18">

</xml_diff>

<commit_message>
new data - 01.03.2023 21:49:28,02
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Часы работы</t>
   </si>
@@ -220,9 +220,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -270,6 +267,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -660,26 +660,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ20"/>
+  <dimension ref="A1:AMJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="17" style="8" customWidth="1"/>
-    <col min="3" max="33" width="9" style="8" customWidth="1"/>
-    <col min="34" max="34" width="17.7109375" style="8" customWidth="1"/>
-    <col min="35" max="35" width="16.140625" style="8" customWidth="1"/>
-    <col min="36" max="36" width="16.85546875" style="8" customWidth="1"/>
-    <col min="37" max="37" width="21.85546875" style="8" customWidth="1"/>
-    <col min="38" max="38" width="20" style="8" customWidth="1"/>
-    <col min="39" max="39" width="27.28515625" style="8" customWidth="1"/>
-    <col min="40" max="64" width="9" style="8" customWidth="1"/>
-    <col min="65" max="1024" width="11.85546875" style="8"/>
-    <col min="1025" max="16384" width="11.85546875" style="10"/>
+    <col min="1" max="1" width="19.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17" style="7" customWidth="1"/>
+    <col min="3" max="33" width="9" style="7" customWidth="1"/>
+    <col min="34" max="34" width="17.7109375" style="7" customWidth="1"/>
+    <col min="35" max="35" width="16.140625" style="7" customWidth="1"/>
+    <col min="36" max="36" width="16.85546875" style="7" customWidth="1"/>
+    <col min="37" max="37" width="21.85546875" style="7" customWidth="1"/>
+    <col min="38" max="38" width="20" style="7" customWidth="1"/>
+    <col min="39" max="39" width="27.28515625" style="7" customWidth="1"/>
+    <col min="40" max="64" width="9" style="7" customWidth="1"/>
+    <col min="65" max="1024" width="11.85546875" style="7"/>
+    <col min="1025" max="16384" width="11.85546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
@@ -720,121 +720,121 @@
       <c r="AG1" s="25"/>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>1</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>2</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>3</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <v>4</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="11">
         <v>5</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="11">
         <v>6</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="11">
         <v>7</v>
       </c>
-      <c r="J2" s="12">
-        <v>8</v>
-      </c>
-      <c r="K2" s="12">
+      <c r="J2" s="11">
+        <v>8</v>
+      </c>
+      <c r="K2" s="11">
         <v>9</v>
       </c>
-      <c r="L2" s="12">
+      <c r="L2" s="11">
         <v>10</v>
       </c>
-      <c r="M2" s="12">
+      <c r="M2" s="11">
         <v>11</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="11">
         <v>12</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="11">
         <v>13</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="11">
         <v>14</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="Q2" s="11">
         <v>15</v>
       </c>
-      <c r="R2" s="12">
+      <c r="R2" s="11">
         <v>16</v>
       </c>
-      <c r="S2" s="12">
+      <c r="S2" s="11">
         <v>17</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="11">
         <v>18</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="11">
         <v>19</v>
       </c>
-      <c r="V2" s="12">
+      <c r="V2" s="11">
         <v>20</v>
       </c>
-      <c r="W2" s="12">
+      <c r="W2" s="11">
         <v>21</v>
       </c>
-      <c r="X2" s="12">
+      <c r="X2" s="11">
         <v>22</v>
       </c>
-      <c r="Y2" s="12">
+      <c r="Y2" s="11">
         <v>23</v>
       </c>
-      <c r="Z2" s="12">
+      <c r="Z2" s="11">
         <v>24</v>
       </c>
-      <c r="AA2" s="12">
+      <c r="AA2" s="11">
         <v>25</v>
       </c>
-      <c r="AB2" s="12">
+      <c r="AB2" s="11">
         <v>26</v>
       </c>
-      <c r="AC2" s="12">
+      <c r="AC2" s="11">
         <v>27</v>
       </c>
-      <c r="AD2" s="12">
+      <c r="AD2" s="11">
         <v>28</v>
       </c>
-      <c r="AE2" s="12">
+      <c r="AE2" s="11">
         <v>29</v>
       </c>
-      <c r="AF2" s="12">
+      <c r="AF2" s="11">
         <v>30</v>
       </c>
-      <c r="AG2" s="12">
+      <c r="AG2" s="11">
         <v>31</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AH2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="AI2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="13" t="s">
+      <c r="AJ2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" s="14" t="s">
+      <c r="AK2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AM2" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -851,10 +851,10 @@
       <c r="D4" s="2">
         <v>8</v>
       </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7">
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
         <v>0</v>
       </c>
       <c r="G4" s="2">
@@ -872,10 +872,10 @@
       <c r="K4" s="2">
         <v>8</v>
       </c>
-      <c r="L4" s="16">
-        <v>0</v>
-      </c>
-      <c r="M4" s="16">
+      <c r="L4" s="15">
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
         <v>0</v>
       </c>
       <c r="N4" s="2">
@@ -893,10 +893,10 @@
       <c r="R4" s="2">
         <v>8</v>
       </c>
-      <c r="S4" s="7">
-        <v>0</v>
-      </c>
-      <c r="T4" s="7">
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6">
         <v>0</v>
       </c>
       <c r="U4" s="2">
@@ -914,10 +914,10 @@
       <c r="Y4" s="2">
         <v>8</v>
       </c>
-      <c r="Z4" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="7">
+      <c r="Z4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="6">
         <v>0</v>
       </c>
       <c r="AB4" s="2">
@@ -938,11 +938,11 @@
       <c r="AG4" s="5">
         <v>0</v>
       </c>
-      <c r="AH4" s="17">
+      <c r="AH4" s="16">
         <f>SUM($C4:$AG4)</f>
         <v>176</v>
       </c>
-      <c r="AI4" s="18">
+      <c r="AI4" s="17">
         <f>(AH4-AH5)</f>
         <v>58.749999999999986</v>
       </c>
@@ -954,7 +954,7 @@
         <f>AH4*$AL4</f>
         <v>21120</v>
       </c>
-      <c r="AL4" s="19">
+      <c r="AL4" s="18">
         <v>120</v>
       </c>
     </row>
@@ -968,10 +968,10 @@
       <c r="D5" s="2">
         <v>8</v>
       </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
         <v>0</v>
       </c>
       <c r="G5" s="2">
@@ -989,10 +989,10 @@
       <c r="K5" s="2">
         <v>6.2</v>
       </c>
-      <c r="L5" s="16">
-        <v>0</v>
-      </c>
-      <c r="M5" s="16">
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
         <v>0</v>
       </c>
       <c r="N5" s="2">
@@ -1010,10 +1010,10 @@
       <c r="R5" s="2">
         <v>5.8</v>
       </c>
-      <c r="S5" s="7">
-        <v>0</v>
-      </c>
-      <c r="T5" s="7">
+      <c r="S5" s="6">
+        <v>0</v>
+      </c>
+      <c r="T5" s="6">
         <v>0</v>
       </c>
       <c r="U5" s="2">
@@ -1031,10 +1031,10 @@
       <c r="Y5" s="2">
         <v>8</v>
       </c>
-      <c r="Z5" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="7">
+      <c r="Z5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="6">
         <v>1</v>
       </c>
       <c r="AB5" s="2">
@@ -1055,11 +1055,11 @@
       <c r="AG5" s="5">
         <v>0</v>
       </c>
-      <c r="AH5" s="17">
+      <c r="AH5" s="16">
         <f>SUM($C5:$AG5)</f>
         <v>117.25000000000001</v>
       </c>
-      <c r="AI5" s="18">
+      <c r="AI5" s="17">
         <f>(AI4*$AL4)</f>
         <v>7049.9999999999982</v>
       </c>
@@ -1079,10 +1079,10 @@
       <c r="D7" s="5">
         <v>0</v>
       </c>
-      <c r="E7" s="6">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="E7" s="23">
+        <v>8</v>
+      </c>
+      <c r="F7" s="23">
         <v>8</v>
       </c>
       <c r="G7" s="2">
@@ -1121,10 +1121,10 @@
       <c r="R7" s="5">
         <v>0</v>
       </c>
-      <c r="S7" s="6">
-        <v>8</v>
-      </c>
-      <c r="T7" s="6">
+      <c r="S7" s="23">
+        <v>8</v>
+      </c>
+      <c r="T7" s="23">
         <v>8</v>
       </c>
       <c r="U7" s="2">
@@ -1142,10 +1142,10 @@
       <c r="Y7" s="5">
         <v>0</v>
       </c>
-      <c r="Z7" s="6">
-        <v>8</v>
-      </c>
-      <c r="AA7" s="6">
+      <c r="Z7" s="23">
+        <v>8</v>
+      </c>
+      <c r="AA7" s="23">
         <v>8</v>
       </c>
       <c r="AB7" s="2">
@@ -1166,11 +1166,11 @@
       <c r="AG7" s="2">
         <v>8</v>
       </c>
-      <c r="AH7" s="17">
+      <c r="AH7" s="16">
         <f>SUM($C7:$AG7)</f>
         <v>168</v>
       </c>
-      <c r="AI7" s="18">
+      <c r="AI7" s="17">
         <f>(AH7-AH8)</f>
         <v>58.7</v>
       </c>
@@ -1197,10 +1197,10 @@
       <c r="D8" s="5">
         <v>0</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="23">
         <v>6</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="23">
         <v>5.6</v>
       </c>
       <c r="G8" s="2">
@@ -1239,10 +1239,10 @@
       <c r="R8" s="5">
         <v>0</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="23">
         <v>5</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="23">
         <v>4</v>
       </c>
       <c r="U8" s="2">
@@ -1260,10 +1260,10 @@
       <c r="Y8" s="5">
         <v>0</v>
       </c>
-      <c r="Z8" s="6">
+      <c r="Z8" s="23">
         <v>5.7</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AA8" s="23">
         <v>4.7</v>
       </c>
       <c r="AB8" s="2">
@@ -1284,11 +1284,11 @@
       <c r="AG8" s="2">
         <v>5.5</v>
       </c>
-      <c r="AH8" s="17">
+      <c r="AH8" s="16">
         <f>SUM($C8:$AG8)</f>
         <v>109.3</v>
       </c>
-      <c r="AI8" s="18">
+      <c r="AI8" s="17">
         <f>(AI7*$AL4)</f>
         <v>7044</v>
       </c>
@@ -1309,10 +1309,10 @@
       <c r="D10" s="2">
         <v>8</v>
       </c>
-      <c r="E10" s="6">
-        <v>8</v>
-      </c>
-      <c r="F10" s="20">
+      <c r="E10" s="23">
+        <v>8</v>
+      </c>
+      <c r="F10" s="19">
         <v>0</v>
       </c>
       <c r="G10" s="5">
@@ -1351,10 +1351,10 @@
       <c r="R10" s="2">
         <v>8</v>
       </c>
-      <c r="S10" s="6">
-        <v>8</v>
-      </c>
-      <c r="T10" s="6">
+      <c r="S10" s="23">
+        <v>8</v>
+      </c>
+      <c r="T10" s="23">
         <v>8</v>
       </c>
       <c r="U10" s="5">
@@ -1372,10 +1372,10 @@
       <c r="Y10" s="2">
         <v>8</v>
       </c>
-      <c r="Z10" s="6">
-        <v>8</v>
-      </c>
-      <c r="AA10" s="6">
+      <c r="Z10" s="23">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="23">
         <v>8</v>
       </c>
       <c r="AB10" s="5">
@@ -1394,11 +1394,11 @@
         <v>8</v>
       </c>
       <c r="AG10" s="2"/>
-      <c r="AH10" s="17">
+      <c r="AH10" s="16">
         <f>SUM($C10:$AG10)</f>
         <v>168</v>
       </c>
-      <c r="AI10" s="18">
+      <c r="AI10" s="17">
         <f>(AH10-AH11)</f>
         <v>62.300000000000011</v>
       </c>
@@ -1425,10 +1425,10 @@
       <c r="D11" s="2">
         <v>6</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="23">
         <v>3.3</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F11" s="19">
         <v>0</v>
       </c>
       <c r="G11" s="5">
@@ -1467,10 +1467,10 @@
       <c r="R11" s="2">
         <v>6.5</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="23">
         <v>5</v>
       </c>
-      <c r="T11" s="6">
+      <c r="T11" s="23">
         <v>6</v>
       </c>
       <c r="U11" s="5">
@@ -1488,10 +1488,10 @@
       <c r="Y11" s="2">
         <v>6</v>
       </c>
-      <c r="Z11" s="6">
+      <c r="Z11" s="23">
         <v>4</v>
       </c>
-      <c r="AA11" s="6">
+      <c r="AA11" s="23">
         <v>4</v>
       </c>
       <c r="AB11" s="5">
@@ -1510,11 +1510,11 @@
         <v>6</v>
       </c>
       <c r="AG11" s="2"/>
-      <c r="AH11" s="17">
+      <c r="AH11" s="16">
         <f>SUM($C11:$AG11)</f>
         <v>105.69999999999999</v>
       </c>
-      <c r="AI11" s="18">
+      <c r="AI11" s="17">
         <f>(AI10*$AL4)</f>
         <v>7476.0000000000018</v>
       </c>
@@ -1577,10 +1577,10 @@
       <c r="R13" s="2">
         <v>8</v>
       </c>
-      <c r="S13" s="7">
-        <v>0</v>
-      </c>
-      <c r="T13" s="7">
+      <c r="S13" s="6">
+        <v>0</v>
+      </c>
+      <c r="T13" s="6">
         <v>0</v>
       </c>
       <c r="U13" s="2">
@@ -1598,10 +1598,10 @@
       <c r="Y13" s="2">
         <v>8</v>
       </c>
-      <c r="Z13" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="7">
+      <c r="Z13" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="6">
         <v>0</v>
       </c>
       <c r="AB13" s="2">
@@ -1622,11 +1622,11 @@
       <c r="AG13" s="5">
         <v>0</v>
       </c>
-      <c r="AH13" s="17">
+      <c r="AH13" s="16">
         <f>SUM($C13:$AG13)</f>
         <v>176</v>
       </c>
-      <c r="AI13" s="18">
+      <c r="AI13" s="17">
         <f>(AH13-AH14)</f>
         <v>91</v>
       </c>
@@ -1695,10 +1695,10 @@
       <c r="R14" s="2">
         <v>6</v>
       </c>
-      <c r="S14" s="7">
-        <v>0</v>
-      </c>
-      <c r="T14" s="7">
+      <c r="S14" s="6">
+        <v>0</v>
+      </c>
+      <c r="T14" s="6">
         <v>0</v>
       </c>
       <c r="U14" s="2">
@@ -1716,10 +1716,10 @@
       <c r="Y14" s="2">
         <v>3</v>
       </c>
-      <c r="Z14" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="7">
+      <c r="Z14" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="6">
         <v>0</v>
       </c>
       <c r="AB14" s="2">
@@ -1740,11 +1740,11 @@
       <c r="AG14" s="5">
         <v>0</v>
       </c>
-      <c r="AH14" s="17">
+      <c r="AH14" s="16">
         <f>SUM($C14:$AG14)</f>
         <v>85</v>
       </c>
-      <c r="AI14" s="18">
+      <c r="AI14" s="17">
         <f>(AI13*$AL$4)</f>
         <v>10920</v>
       </c>
@@ -1807,10 +1807,10 @@
       <c r="R16" s="2">
         <v>8</v>
       </c>
-      <c r="S16" s="6">
-        <v>8</v>
-      </c>
-      <c r="T16" s="6">
+      <c r="S16" s="23">
+        <v>8</v>
+      </c>
+      <c r="T16" s="23">
         <v>8</v>
       </c>
       <c r="U16" s="2">
@@ -1828,10 +1828,10 @@
       <c r="Y16" s="2">
         <v>8</v>
       </c>
-      <c r="Z16" s="6">
-        <v>8</v>
-      </c>
-      <c r="AA16" s="6">
+      <c r="Z16" s="23">
+        <v>8</v>
+      </c>
+      <c r="AA16" s="23">
         <v>8</v>
       </c>
       <c r="AB16" s="2">
@@ -1852,11 +1852,11 @@
       <c r="AG16" s="2">
         <v>8</v>
       </c>
-      <c r="AH16" s="17">
+      <c r="AH16" s="16">
         <f>SUM($C16:$AG16)</f>
         <v>136</v>
       </c>
-      <c r="AI16" s="18">
+      <c r="AI16" s="17">
         <f>(AH16-AH17)</f>
         <v>33.5</v>
       </c>
@@ -1970,11 +1970,11 @@
       <c r="AG17" s="2">
         <v>8</v>
       </c>
-      <c r="AH17" s="17">
+      <c r="AH17" s="16">
         <f>SUM($C17:$AG17)</f>
         <v>102.5</v>
       </c>
-      <c r="AI17" s="18">
+      <c r="AI17" s="17">
         <f>(AI16*$AL$4)</f>
         <v>4020</v>
       </c>
@@ -2037,10 +2037,10 @@
       <c r="R19" s="2">
         <v>8</v>
       </c>
-      <c r="S19" s="6">
-        <v>8</v>
-      </c>
-      <c r="T19" s="7">
+      <c r="S19" s="23">
+        <v>8</v>
+      </c>
+      <c r="T19" s="6">
         <v>0</v>
       </c>
       <c r="U19" s="5">
@@ -2055,13 +2055,13 @@
       <c r="X19" s="2">
         <v>8</v>
       </c>
-      <c r="Y19" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="7">
+      <c r="Y19" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="6">
         <v>0</v>
       </c>
       <c r="AB19" s="5">
@@ -2076,17 +2076,17 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
-      <c r="AH19" s="17">
+      <c r="AH19" s="16">
         <f>SUM($C19:$AG19)</f>
         <v>144</v>
       </c>
-      <c r="AI19" s="18">
+      <c r="AI19" s="17">
         <f>(AH19-AH20)</f>
-        <v>92</v>
+        <v>81.5</v>
       </c>
       <c r="AJ19" s="24">
         <f>(AH20*$AL$4)</f>
-        <v>6240</v>
+        <v>7500</v>
       </c>
       <c r="AK19" s="24">
         <f>AH19*$AL$4</f>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="AM19" s="24">
         <f>AJ19+5000</f>
-        <v>11240</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
@@ -2116,19 +2116,19 @@
       <c r="G20" s="5">
         <v>0</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>4</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>4</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>4</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="8">
         <v>4</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>4</v>
       </c>
       <c r="M20" s="5">
@@ -2149,10 +2149,10 @@
       <c r="R20" s="2">
         <v>0</v>
       </c>
-      <c r="S20" s="6">
-        <v>0</v>
-      </c>
-      <c r="T20" s="7">
+      <c r="S20" s="23">
+        <v>0</v>
+      </c>
+      <c r="T20" s="6">
         <v>0</v>
       </c>
       <c r="U20" s="5">
@@ -2164,38 +2164,211 @@
       <c r="W20" s="2">
         <v>5</v>
       </c>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="7">
+      <c r="X20" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y20" s="20">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="21">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="6">
         <v>0</v>
       </c>
       <c r="AB20" s="5">
         <v>0</v>
       </c>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
+      <c r="AC20" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>3.5</v>
+      </c>
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
-      <c r="AH20" s="17">
+      <c r="AH20" s="16">
         <f>SUM($C20:$AG20)</f>
-        <v>52</v>
-      </c>
-      <c r="AI20" s="18">
+        <v>62.5</v>
+      </c>
+      <c r="AI20" s="17">
         <f>(AI19*$AL$4)</f>
-        <v>11040</v>
+        <v>9780</v>
       </c>
       <c r="AJ20" s="24"/>
       <c r="AK20" s="24"/>
       <c r="AM20" s="24"/>
     </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <v>8</v>
+      </c>
+      <c r="D22" s="2">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3">
+        <v>8</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>8</v>
+      </c>
+      <c r="I22" s="2">
+        <v>8</v>
+      </c>
+      <c r="J22" s="2">
+        <v>8</v>
+      </c>
+      <c r="K22" s="2">
+        <v>8</v>
+      </c>
+      <c r="L22" s="2">
+        <v>8</v>
+      </c>
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
+        <v>8</v>
+      </c>
+      <c r="P22" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>8</v>
+      </c>
+      <c r="R22" s="2">
+        <v>8</v>
+      </c>
+      <c r="S22" s="23">
+        <v>8</v>
+      </c>
+      <c r="T22" s="6">
+        <v>0</v>
+      </c>
+      <c r="U22" s="5">
+        <v>0</v>
+      </c>
+      <c r="V22" s="2">
+        <v>8</v>
+      </c>
+      <c r="W22" s="2">
+        <v>8</v>
+      </c>
+      <c r="X22" s="2">
+        <v>8</v>
+      </c>
+      <c r="Y22" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>8</v>
+      </c>
+      <c r="AD22" s="2">
+        <v>8</v>
+      </c>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="16">
+        <f>SUM($C22:$AG22)</f>
+        <v>144</v>
+      </c>
+      <c r="AI22" s="17">
+        <f>(AH22-AH23)</f>
+        <v>137.5</v>
+      </c>
+      <c r="AJ22" s="24">
+        <f>(AH23*$AL$4)</f>
+        <v>780</v>
+      </c>
+      <c r="AK22" s="24">
+        <f>AH22*$AL$4</f>
+        <v>17280</v>
+      </c>
+      <c r="AM22" s="24">
+        <f>AJ22+5000</f>
+        <v>5780</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="16">
+        <f>SUM($C23:$AG23)</f>
+        <v>6.5</v>
+      </c>
+      <c r="AI23" s="17">
+        <f>(AI22*$AL$4)</f>
+        <v>16500</v>
+      </c>
+      <c r="AJ23" s="24"/>
+      <c r="AK23" s="24"/>
+      <c r="AM23" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK22:AK23"/>
+    <mergeCell ref="AM22:AM23"/>
     <mergeCell ref="A1:AG1"/>
     <mergeCell ref="AJ4:AJ5"/>
     <mergeCell ref="AK4:AK5"/>
@@ -2216,6 +2389,6 @@
     <mergeCell ref="AM19:AM20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new data - 03.03.2023 21:58:34,02
</commit_message>
<xml_diff>
--- a/часы.xlsx
+++ b/часы.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilya\Desktop\table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilyab\Desktop\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2634054-032F-4394-B213-1201541D6E23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Парақ1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -102,7 +103,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,8 +176,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -199,11 +206,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -276,6 +337,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -659,11 +738,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI20" sqref="AI20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J29" sqref="J28:J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,11 +2352,11 @@
       <c r="X22" s="2">
         <v>8</v>
       </c>
-      <c r="Y22" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="22">
-        <v>0</v>
+      <c r="Y22" s="30">
+        <v>8</v>
+      </c>
+      <c r="Z22" s="27">
+        <v>8</v>
       </c>
       <c r="AA22" s="6">
         <v>0</v>
@@ -2291,28 +2370,34 @@
       <c r="AD22" s="2">
         <v>8</v>
       </c>
-      <c r="AE22" s="2"/>
-      <c r="AF22" s="2"/>
-      <c r="AG22" s="2"/>
+      <c r="AE22" s="2">
+        <v>8</v>
+      </c>
+      <c r="AF22" s="2">
+        <v>8</v>
+      </c>
+      <c r="AG22" s="2">
+        <v>8</v>
+      </c>
       <c r="AH22" s="16">
         <f>SUM($C22:$AG22)</f>
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AI22" s="17">
         <f>(AH22-AH23)</f>
-        <v>137.5</v>
+        <v>167.2</v>
       </c>
       <c r="AJ22" s="24">
         <f>(AH23*$AL$4)</f>
-        <v>780</v>
+        <v>2016</v>
       </c>
       <c r="AK22" s="24">
         <f>AH22*$AL$4</f>
-        <v>17280</v>
+        <v>22080</v>
       </c>
       <c r="AM22" s="24">
         <f>AJ22+5000</f>
-        <v>5780</v>
+        <v>7016</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
@@ -2322,15 +2407,19 @@
       <c r="C23" s="2">
         <v>6.5</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="E23" s="3">
+        <v>5</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="2"/>
@@ -2342,9 +2431,9 @@
       <c r="U23" s="5"/>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
-      <c r="X23" s="2"/>
-      <c r="Y23" s="20"/>
-      <c r="Z23" s="21"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="29"/>
       <c r="AA23" s="6"/>
       <c r="AB23" s="5"/>
       <c r="AC23" s="2"/>
@@ -2354,11 +2443,11 @@
       <c r="AG23" s="2"/>
       <c r="AH23" s="16">
         <f>SUM($C23:$AG23)</f>
-        <v>6.5</v>
+        <v>16.8</v>
       </c>
       <c r="AI23" s="17">
         <f>(AI22*$AL$4)</f>
-        <v>16500</v>
+        <v>20064</v>
       </c>
       <c r="AJ23" s="24"/>
       <c r="AK23" s="24"/>
@@ -2366,6 +2455,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AK16:AK17"/>
+    <mergeCell ref="AM16:AM17"/>
+    <mergeCell ref="AJ19:AJ20"/>
+    <mergeCell ref="AK19:AK20"/>
+    <mergeCell ref="AM19:AM20"/>
     <mergeCell ref="AJ22:AJ23"/>
     <mergeCell ref="AK22:AK23"/>
     <mergeCell ref="AM22:AM23"/>
@@ -2382,11 +2476,6 @@
     <mergeCell ref="AK13:AK14"/>
     <mergeCell ref="AM13:AM14"/>
     <mergeCell ref="AJ16:AJ17"/>
-    <mergeCell ref="AK16:AK17"/>
-    <mergeCell ref="AM16:AM17"/>
-    <mergeCell ref="AJ19:AJ20"/>
-    <mergeCell ref="AK19:AK20"/>
-    <mergeCell ref="AM19:AM20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>